<commit_message>
FEAT:Update Optuna for mlp
</commit_message>
<xml_diff>
--- a/final_project/Metric.xlsx
+++ b/final_project/Metric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\22-1_multivariate\final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877A76F1-7033-48DC-AECF-BCB05457D63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203FB4E3-A40F-4C43-BBAB-4146A61409AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{387F913E-4B8E-4F70-9082-430D9D091FEF}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="23040" windowHeight="12204" activeTab="3" xr2:uid="{387F913E-4B8E-4F70-9082-430D9D091FEF}"/>
   </bookViews>
   <sheets>
     <sheet name="specificity" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="25">
   <si>
     <t>logistic regression</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -83,12 +83,60 @@
     <t>baseline(37)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>38 (Base)</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>MLP</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>Ensemble</t>
+  </si>
+  <si>
+    <t>17 *</t>
+  </si>
+  <si>
+    <t>LR -stat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF -stat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GB -stat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MLP -stat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SVM -stat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ensemble -stat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +180,15 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -161,7 +218,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -178,6 +235,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3942,6 +4008,9 @@
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-14C6-497F-8CC5-937A4EE7C7B1}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4976,6 +5045,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-4247-45CE-A9B8-8567A3EF1C21}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5465,7 +5537,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>AUC!$B$14</c:f>
+              <c:f>AUC!$B$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5500,7 +5572,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>AUC!$C$13:$G$13</c:f>
+              <c:f>AUC!$C$22:$G$22</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -5523,7 +5595,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>AUC!$C$14:$G$14</c:f>
+              <c:f>AUC!$C$23:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5557,7 +5629,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>AUC!$B$15</c:f>
+              <c:f>AUC!$B$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5607,6 +5679,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-188C-4FC7-BA38-7D54CB34A806}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -5687,7 +5762,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>AUC!$C$13:$G$13</c:f>
+              <c:f>AUC!$C$22:$G$22</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -5710,7 +5785,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>AUC!$C$15:$G$15</c:f>
+              <c:f>AUC!$C$24:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5744,7 +5819,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>AUC!$B$16</c:f>
+              <c:f>AUC!$B$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5779,7 +5854,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>AUC!$C$13:$G$13</c:f>
+              <c:f>AUC!$C$22:$G$22</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -5802,7 +5877,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>AUC!$C$16:$G$16</c:f>
+              <c:f>AUC!$C$25:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5836,7 +5911,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>AUC!$B$17</c:f>
+              <c:f>AUC!$B$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5873,7 +5948,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>AUC!$C$13:$G$13</c:f>
+              <c:f>AUC!$C$22:$G$22</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -5896,7 +5971,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>AUC!$C$17:$G$17</c:f>
+              <c:f>AUC!$C$26:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5930,7 +6005,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>AUC!$B$18</c:f>
+              <c:f>AUC!$B$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6059,7 +6134,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>AUC!$C$13:$G$13</c:f>
+              <c:f>AUC!$C$22:$G$22</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -6082,7 +6157,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>AUC!$C$18:$G$18</c:f>
+              <c:f>AUC!$C$27:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -6116,7 +6191,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>AUC!$B$19</c:f>
+              <c:f>AUC!$B$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6153,7 +6228,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>AUC!$C$13:$G$13</c:f>
+              <c:f>AUC!$C$22:$G$22</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -6176,7 +6251,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>AUC!$C$19:$G$19</c:f>
+              <c:f>AUC!$C$28:$G$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -6335,6 +6410,1641 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:t>AUC</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.6665124630609402E-2"/>
+          <c:y val="0.13525643817898506"/>
+          <c:w val="0.925515168429204"/>
+          <c:h val="0.69073808903181233"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AUC!$B$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>AUC!$C$32:$I$32</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38 (Base)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AUC!$C$33:$I$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.70250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.69940000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69620000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.69479999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.66859999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.66359999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C6A6-4275-A1F9-296FA59F4192}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AUC!$B$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>AUC!$C$32:$I$32</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38 (Base)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AUC!$C$34:$I$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.70199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.67020000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.67020000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.69148900000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.76180000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C6A6-4275-A1F9-296FA59F4192}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AUC!$B$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>AUC!$C$32:$I$32</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38 (Base)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AUC!$C$35:$I$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.70209999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68079999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7127</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.70209999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.69140000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.69140000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.70209999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C6A6-4275-A1F9-296FA59F4192}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AUC!$B$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MLP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>AUC!$C$32:$I$32</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38 (Base)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AUC!$C$36:$I$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.73329999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71860000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7329</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.72809999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.70340000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.63329999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.64639999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-C6A6-4275-A1F9-296FA59F4192}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AUC!$B$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.2356243248002569E-2"/>
+                  <c:y val="-2.3952642921627288E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-C6A6-4275-A1F9-296FA59F4192}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ko-KR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>AUC!$C$32:$I$32</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38 (Base)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AUC!$C$37:$I$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.75319999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.74780000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75139999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.74550000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.77500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.76590000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.75960000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-C6A6-4275-A1F9-296FA59F4192}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AUC!$B$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ensemble</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>AUC!$C$32:$I$32</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38 (Base)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AUC!$C$38:$I$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.73240000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76319999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.77039999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76949999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.74729999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.72650000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.68620000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-C6A6-4275-A1F9-296FA59F4192}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AUC!$B$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LR -stat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>AUC!$C$32:$I$32</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38 (Base)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AUC!$C$39:$I$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.72470000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70520000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.68889999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.68889999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.68889999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.68889999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.66359999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-C6A6-4275-A1F9-296FA59F4192}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AUC!$B$40</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RF -stat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>AUC!$C$32:$I$32</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38 (Base)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AUC!$C$40:$I$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.69140000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-C6A6-4275-A1F9-296FA59F4192}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AUC!$B$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GB -stat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>AUC!$C$32:$I$32</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38 (Base)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AUC!$C$41:$I$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.70209999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68079999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7127</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7127</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7127</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7127</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.70209999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-C6A6-4275-A1F9-296FA59F4192}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AUC!$B$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MLP -stat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>AUC!$C$32:$I$32</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38 (Base)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AUC!$C$42:$I$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.75260000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.73540000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.746</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.746</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.746</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.746</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.64639999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-C6A6-4275-A1F9-296FA59F4192}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AUC!$B$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SVM -stat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-C6A6-4275-A1F9-296FA59F4192}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ko-KR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>AUC!$C$32:$I$32</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38 (Base)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AUC!$C$43:$I$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.74460000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7127</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.70199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.70199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.70199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.75960000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-C6A6-4275-A1F9-296FA59F4192}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AUC!$B$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ensemble -stat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.8485565115767072E-2"/>
+                  <c:y val="-2.3611092462318847E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-4182-43A4-9FF1-7D2025D2903D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ko-KR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>AUC!$C$32:$I$32</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38 (Base)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AUC!$C$44:$I$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.74919999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77090000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7863</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7863</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7863</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7863</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.68620000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-C6A6-4275-A1F9-296FA59F4192}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="696418528"/>
+        <c:axId val="696419360"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="696418528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="696419360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="696419360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.60000000000000009"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="696418528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.1149106129638728E-2"/>
+          <c:y val="0.87083492995685774"/>
+          <c:w val="0.94018373504422637"/>
+          <c:h val="0.12280205621009944"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6728,6 +8438,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -10412,6 +12162,522 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -11040,16 +13306,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>43960</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>80427</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>465303</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>35604</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>646485</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>395474</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>209774</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11069,6 +13335,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>663387</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>178010</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>88366</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="차트 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65758966-3E6E-BDDA-ACC1-C08D62694326}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -11376,7 +13678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DEC605-0B52-44C8-B566-84FB2ED1CCE6}">
   <dimension ref="A2:AG22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -12444,10 +14746,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57290BA2-B033-4EDB-8465-0445A2C8ADE5}">
-  <dimension ref="B2:G19"/>
+  <dimension ref="B2:I44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -12456,295 +14758,777 @@
     <col min="7" max="7" width="13.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="D2" s="6">
         <v>15</v>
       </c>
-      <c r="F2">
+      <c r="E2" s="6">
+        <v>17</v>
+      </c>
+      <c r="F2" s="6">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
-        <v>3</v>
+      <c r="G2" s="6">
+        <v>25</v>
+      </c>
+      <c r="H2" s="6">
+        <v>30</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B3" t="s">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0.70250000000000001</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.69940000000000002</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.69620000000000004</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.7016</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0.69479999999999997</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0.66859999999999997</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0.66359999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0.67020000000000002</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0.76</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0.67020000000000002</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0.69148900000000002</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0.76180000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.70209999999999995</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.68079999999999996</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0.7127</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.70209999999999995</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0.69140000000000001</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0.69140000000000001</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0.70209999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.73329999999999995</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.71860000000000002</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0.7329</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0.72809999999999997</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.70340000000000003</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0.63329999999999997</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0.64639999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.75319999999999998</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.74780000000000002</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.75139999999999996</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.74550000000000005</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0.76590000000000003</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0.75960000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.73240000000000005</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.76319999999999999</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0.77039999999999997</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.76949999999999996</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0.74729999999999996</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0.72650000000000003</v>
+      </c>
+      <c r="I8" s="7">
+        <v>0.68620000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6">
+        <v>10</v>
+      </c>
+      <c r="D10" s="6">
+        <v>15</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.72470000000000001</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0.70520000000000005</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0.68889999999999996</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0.66359999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0.67</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.66</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0.68</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0.69140000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0.70209999999999995</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0.68079999999999996</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0.7127</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0.70209999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.75260000000000005</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0.73540000000000005</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.746</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0.64639999999999997</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.74460000000000004</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0.7127</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.75960000000000005</v>
+      </c>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.74919999999999998</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0.77090000000000003</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0.7863</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0.68620000000000003</v>
+      </c>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>15</v>
+      </c>
+      <c r="E22">
+        <v>17</v>
+      </c>
+      <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B23" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C23" s="1">
+        <v>0.70250000000000001</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.69940000000000002</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.69940000000000002</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.7016</v>
+      </c>
+      <c r="G23" s="1">
         <v>0.66359999999999997</v>
       </c>
-      <c r="D3" s="1">
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.75319999999999998</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.74780000000000002</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.74780000000000002</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.74550000000000005</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.75960000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.76</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.76180000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.72470000000000001</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.70520000000000005</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.68889999999999996</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.68889999999999996</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.66359999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.74460000000000004</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.7127</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.75960000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.69140000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B32" s="6"/>
+      <c r="C32" s="6">
+        <v>10</v>
+      </c>
+      <c r="D32" s="6">
+        <v>15</v>
+      </c>
+      <c r="E32" s="6">
+        <v>17</v>
+      </c>
+      <c r="F32" s="6">
+        <v>20</v>
+      </c>
+      <c r="G32" s="6">
+        <v>25</v>
+      </c>
+      <c r="H32" s="6">
+        <v>30</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B33" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="7">
         <v>0.70250000000000001</v>
       </c>
-      <c r="E3" s="1">
+      <c r="D33" s="7">
         <v>0.69940000000000002</v>
       </c>
-      <c r="F3" s="1">
+      <c r="E33" s="7">
+        <v>0.69620000000000004</v>
+      </c>
+      <c r="F33" s="7">
         <v>0.7016</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G33" s="7">
+        <v>0.69479999999999997</v>
+      </c>
+      <c r="H33" s="7">
+        <v>0.66859999999999997</v>
+      </c>
+      <c r="I33" s="7">
         <v>0.66359999999999997</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="7">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="D34" s="7">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="E34" s="7">
+        <v>0.67020000000000002</v>
+      </c>
+      <c r="F34" s="7">
+        <v>0.76</v>
+      </c>
+      <c r="G34" s="7">
+        <v>0.67020000000000002</v>
+      </c>
+      <c r="H34" s="7">
+        <v>0.69148900000000002</v>
+      </c>
+      <c r="I34" s="7">
+        <v>0.76180000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B35" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="7">
+        <v>0.70209999999999995</v>
+      </c>
+      <c r="D35" s="7">
+        <v>0.68079999999999996</v>
+      </c>
+      <c r="E35" s="7">
+        <v>0.7127</v>
+      </c>
+      <c r="F35" s="7">
+        <v>0.70209999999999995</v>
+      </c>
+      <c r="G35" s="7">
+        <v>0.69140000000000001</v>
+      </c>
+      <c r="H35" s="7">
+        <v>0.69140000000000001</v>
+      </c>
+      <c r="I35" s="7">
+        <v>0.70209999999999995</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B36" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="8">
+        <v>0.73329999999999995</v>
+      </c>
+      <c r="D36" s="7">
+        <v>0.71860000000000002</v>
+      </c>
+      <c r="E36" s="7">
+        <v>0.7329</v>
+      </c>
+      <c r="F36" s="7">
+        <v>0.72809999999999997</v>
+      </c>
+      <c r="G36" s="7">
+        <v>0.70340000000000003</v>
+      </c>
+      <c r="H36" s="7">
+        <v>0.63329999999999997</v>
+      </c>
+      <c r="I36" s="7">
+        <v>0.64639999999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B37" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="8">
+        <v>0.75319999999999998</v>
+      </c>
+      <c r="D37" s="7">
+        <v>0.74780000000000002</v>
+      </c>
+      <c r="E37" s="7">
+        <v>0.75139999999999996</v>
+      </c>
+      <c r="F37" s="7">
+        <v>0.74550000000000005</v>
+      </c>
+      <c r="G37" s="8">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="H37" s="8">
+        <v>0.76590000000000003</v>
+      </c>
+      <c r="I37" s="8">
         <v>0.75960000000000005</v>
       </c>
-      <c r="D4" s="1">
-        <v>0.75319999999999998</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.74780000000000002</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.74550000000000005</v>
-      </c>
-      <c r="G4" s="1">
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B38" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="7">
+        <v>0.73240000000000005</v>
+      </c>
+      <c r="D38" s="7">
+        <v>0.76319999999999999</v>
+      </c>
+      <c r="E38" s="7">
+        <v>0.77039999999999997</v>
+      </c>
+      <c r="F38" s="7">
+        <v>0.76949999999999996</v>
+      </c>
+      <c r="G38" s="7">
+        <v>0.74729999999999996</v>
+      </c>
+      <c r="H38" s="7">
+        <v>0.72650000000000003</v>
+      </c>
+      <c r="I38" s="7">
+        <v>0.68620000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B39" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="8">
+        <v>0.72470000000000001</v>
+      </c>
+      <c r="D39" s="7">
+        <v>0.70520000000000005</v>
+      </c>
+      <c r="E39" s="7">
+        <v>0.68889999999999996</v>
+      </c>
+      <c r="F39" s="7">
+        <v>0.68889999999999996</v>
+      </c>
+      <c r="G39" s="7">
+        <v>0.68889999999999996</v>
+      </c>
+      <c r="H39" s="7">
+        <v>0.68889999999999996</v>
+      </c>
+      <c r="I39" s="7">
+        <v>0.66359999999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B40" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="7">
+        <v>0.67</v>
+      </c>
+      <c r="D40" s="7">
+        <v>0.66</v>
+      </c>
+      <c r="E40" s="7">
+        <v>0.68</v>
+      </c>
+      <c r="F40" s="7">
+        <v>0.68</v>
+      </c>
+      <c r="G40" s="7">
+        <v>0.68</v>
+      </c>
+      <c r="H40" s="7">
+        <v>0.68</v>
+      </c>
+      <c r="I40" s="7">
+        <v>0.69140000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B41" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="7">
+        <v>0.70209999999999995</v>
+      </c>
+      <c r="D41" s="7">
+        <v>0.68079999999999996</v>
+      </c>
+      <c r="E41" s="7">
+        <v>0.7127</v>
+      </c>
+      <c r="F41" s="7">
+        <v>0.7127</v>
+      </c>
+      <c r="G41" s="7">
+        <v>0.7127</v>
+      </c>
+      <c r="H41" s="7">
+        <v>0.7127</v>
+      </c>
+      <c r="I41" s="7">
+        <v>0.70209999999999995</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B42" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="8">
+        <v>0.75260000000000005</v>
+      </c>
+      <c r="D42" s="7">
+        <v>0.73540000000000005</v>
+      </c>
+      <c r="E42" s="7">
+        <v>0.746</v>
+      </c>
+      <c r="F42" s="7">
+        <v>0.746</v>
+      </c>
+      <c r="G42" s="7">
+        <v>0.746</v>
+      </c>
+      <c r="H42" s="7">
+        <v>0.746</v>
+      </c>
+      <c r="I42" s="7">
+        <v>0.64639999999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B43" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="7">
+        <v>0.74460000000000004</v>
+      </c>
+      <c r="D43" s="7">
+        <v>0.7127</v>
+      </c>
+      <c r="E43" s="7">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="F43" s="7">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="G43" s="7">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="H43" s="7">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="I43" s="8">
         <v>0.75960000000000005</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.69140000000000001</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.70199999999999996</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.70199999999999996</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.76</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0.69140000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>10</v>
-      </c>
-      <c r="E8">
-        <v>15</v>
-      </c>
-      <c r="F8">
-        <v>17</v>
-      </c>
-      <c r="G8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.66359999999999997</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.72470000000000001</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.70520000000000005</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.68889999999999996</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.66359999999999997</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.75960000000000005</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.74460000000000004</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.7127</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.70199999999999996</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0.75960000000000005</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.69140000000000001</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.67</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.66</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0.68</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0.69140000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="C13">
-        <v>10</v>
-      </c>
-      <c r="D13">
-        <v>15</v>
-      </c>
-      <c r="E13">
-        <v>17</v>
-      </c>
-      <c r="F13">
-        <v>20</v>
-      </c>
-      <c r="G13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0.70250000000000001</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0.69940000000000002</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0.69940000000000002</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0.7016</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0.66359999999999997</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0.75319999999999998</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.74780000000000002</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0.74780000000000002</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0.74550000000000005</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0.75960000000000005</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0.70199999999999996</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0.70199999999999996</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0.70199999999999996</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0.76</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0.76180000000000003</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0.72470000000000001</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0.70520000000000005</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0.68889999999999996</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0.68889999999999996</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0.66359999999999997</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0.74460000000000004</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0.7127</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0.70199999999999996</v>
-      </c>
-      <c r="F18" s="1">
-        <v>0.70199999999999996</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0.75960000000000005</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0.67</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0.66</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0.68</v>
-      </c>
-      <c r="F19" s="1">
-        <v>0.68</v>
-      </c>
-      <c r="G19" s="1">
-        <v>0.69140000000000001</v>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B44" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="7">
+        <v>0.74919999999999998</v>
+      </c>
+      <c r="D44" s="8">
+        <v>0.77090000000000003</v>
+      </c>
+      <c r="E44" s="8">
+        <v>0.7863</v>
+      </c>
+      <c r="F44" s="8">
+        <v>0.7863</v>
+      </c>
+      <c r="G44" s="8">
+        <v>0.7863</v>
+      </c>
+      <c r="H44" s="8">
+        <v>0.7863</v>
+      </c>
+      <c r="I44" s="7">
+        <v>0.68620000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update MLP SHAP Value, metric
</commit_message>
<xml_diff>
--- a/final_project/Metric.xlsx
+++ b/final_project/Metric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\22-1_multivariate\final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67587A29-5595-4795-8781-0ABCCFA0675E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34679152-614C-46AE-B2C1-E5F20BF61048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{387F913E-4B8E-4F70-9082-430D9D091FEF}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="25">
   <si>
     <t>logistic regression</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -127,6 +127,9 @@
   <si>
     <t>Ensemble -stat</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>17 *</t>
   </si>
 </sst>
 </file>
@@ -1406,8 +1409,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.6050194427264433E-2"/>
-                  <c:y val="3.6628208157374838E-2"/>
+                  <c:x val="-6.142906054413251E-2"/>
+                  <c:y val="1.1618508391740544E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1420,6 +1423,27 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000F-4CE9-4CB1-BE28-45932769D755}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.2298028578812881E-3"/>
+                  <c:y val="-1.9452068702343527E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-2E8A-476E-9DD6-113B60E24F1B}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1557,25 +1581,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.70209999999999995</c:v>
+                  <c:v>0.74419999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.68079999999999996</c:v>
+                  <c:v>0.76229999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7127</c:v>
+                  <c:v>0.75229999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.70209999999999995</c:v>
+                  <c:v>0.74690000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.69140000000000001</c:v>
+                  <c:v>0.73780000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.69140000000000001</c:v>
+                  <c:v>0.71609999999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70209999999999995</c:v>
+                  <c:v>0.72829999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1626,6 +1650,27 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.9217240010338026E-2"/>
+                  <c:y val="3.6125270447209402E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-2E8A-476E-9DD6-113B60E24F1B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:layout>
@@ -1829,6 +1874,37 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.960862000516902E-2"/>
+                  <c:y val="-4.1683004362164752E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-2E8A-476E-9DD6-113B60E24F1B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-2E8A-476E-9DD6-113B60E24F1B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
               <c:layout>
@@ -2265,7 +2341,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>LR -stat</c:v>
+                  <c:v>LR</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2384,7 +2460,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>17 *</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>38 (Base)</c:v>
@@ -2429,7 +2505,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RF -stat</c:v>
+                  <c:v>RF</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2527,7 +2603,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>17 *</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>38 (Base)</c:v>
@@ -2572,7 +2648,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>GB -stat</c:v>
+                  <c:v>GB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2691,7 +2767,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>17 *</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>38 (Base)</c:v>
@@ -2706,16 +2782,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.70209999999999995</c:v>
+                  <c:v>0.73899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.68079999999999996</c:v>
+                  <c:v>0.75370000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7127</c:v>
+                  <c:v>0.75660000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.70209999999999995</c:v>
+                  <c:v>0.72829999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2736,7 +2812,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MLP -stat</c:v>
+                  <c:v>MLP</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2834,7 +2910,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>17 *</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>38 (Base)</c:v>
@@ -2879,7 +2955,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SVM -stat</c:v>
+                  <c:v>SVM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3019,7 +3095,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>17 *</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>38 (Base)</c:v>
@@ -18515,8 +18591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57290BA2-B033-4EDB-8465-0445A2C8ADE5}">
   <dimension ref="B2:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S62" sqref="S62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -18713,8 +18789,8 @@
       <c r="D10" s="6">
         <v>15</v>
       </c>
-      <c r="E10" s="6">
-        <v>17</v>
+      <c r="E10" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>11</v>
@@ -18722,7 +18798,7 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B11" s="7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C11" s="8">
         <v>0.72470000000000001</v>
@@ -18739,7 +18815,7 @@
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B12" s="7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C12" s="7">
         <v>0.67</v>
@@ -18756,24 +18832,24 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B13" s="7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C13" s="7">
-        <v>0.70209999999999995</v>
+        <v>0.73899999999999999</v>
       </c>
       <c r="D13" s="7">
-        <v>0.68079999999999996</v>
+        <v>0.75370000000000004</v>
       </c>
       <c r="E13" s="7">
-        <v>0.7127</v>
+        <v>0.75660000000000005</v>
       </c>
       <c r="F13" s="7">
-        <v>0.70209999999999995</v>
+        <v>0.72829999999999995</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B14" s="7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C14" s="8">
         <v>0.75260000000000005</v>
@@ -18791,7 +18867,7 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B15" s="7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C15" s="7">
         <v>0.74460000000000004</v>
@@ -19337,32 +19413,32 @@
         <v>14</v>
       </c>
       <c r="C63" s="7">
-        <v>0.70209999999999995</v>
+        <v>0.74419999999999997</v>
       </c>
       <c r="D63" s="7">
-        <v>0.68079999999999996</v>
+        <v>0.76229999999999998</v>
       </c>
       <c r="E63" s="7">
-        <v>0.7127</v>
+        <v>0.75229999999999997</v>
       </c>
       <c r="F63" s="7">
-        <v>0.70209999999999995</v>
+        <v>0.74690000000000001</v>
       </c>
       <c r="G63" s="7">
-        <v>0.69140000000000001</v>
+        <v>0.73780000000000001</v>
       </c>
       <c r="H63" s="7">
-        <v>0.69140000000000001</v>
+        <v>0.71609999999999996</v>
       </c>
       <c r="I63" s="7">
-        <v>0.70209999999999995</v>
+        <v>0.72829999999999995</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B64" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C64" s="8">
+      <c r="C64" s="7">
         <v>0.73329999999999995</v>
       </c>
       <c r="D64" s="7">
@@ -19391,13 +19467,13 @@
       <c r="C65" s="8">
         <v>0.75319999999999998</v>
       </c>
-      <c r="D65" s="7">
+      <c r="D65" s="8">
         <v>0.74780000000000002</v>
       </c>
-      <c r="E65" s="7">
+      <c r="E65" s="8">
         <v>0.75139999999999996</v>
       </c>
-      <c r="F65" s="7">
+      <c r="F65" s="8">
         <v>0.74550000000000005</v>
       </c>
       <c r="G65" s="8">

</xml_diff>

<commit_message>
Fix AUC metrics bug
</commit_message>
<xml_diff>
--- a/final_project/Metric.xlsx
+++ b/final_project/Metric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\22-1_multivariate\final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34679152-614C-46AE-B2C1-E5F20BF61048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB756A3-144F-4DDC-B63B-CC24103D2527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{387F913E-4B8E-4F70-9082-430D9D091FEF}"/>
   </bookViews>
@@ -937,6 +937,27 @@
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.6685019149855087E-2"/>
+                  <c:y val="-1.8650864831581012E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-547B-4278-BC18-552059D77641}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
@@ -1185,8 +1206,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-8.4823986887681016E-2"/>
-                  <c:y val="1.0330913726431861E-16"/>
+                  <c:x val="-5.2951466008136265E-2"/>
+                  <c:y val="-3.4162184747929501E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1199,6 +1220,48 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000010-4CE9-4CB1-BE28-45932769D755}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.4632325369097006E-2"/>
+                  <c:y val="1.3322046308272151E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-547B-4278-BC18-552059D77641}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.6948488053645458E-2"/>
+                  <c:y val="1.8650864831581012E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-547B-4278-BC18-552059D77641}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1220,6 +1283,48 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000012-4CE9-4CB1-BE28-45932769D755}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.0790406711371211E-2"/>
+                  <c:y val="-2.1315274093235491E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-547B-4278-BC18-552059D77641}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5159263176677782E-2"/>
+                  <c:y val="-2.3979683354889873E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-547B-4278-BC18-552059D77641}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1336,22 +1441,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.70199999999999996</c:v>
+                  <c:v>0.76229999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.70199999999999996</c:v>
+                  <c:v>0.75819999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.67020000000000002</c:v>
+                  <c:v>0.74919999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.76</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.67020000000000002</c:v>
+                  <c:v>0.75370000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.69148900000000002</c:v>
+                  <c:v>0.75139999999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.76180000000000003</c:v>
@@ -1427,11 +1532,32 @@
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.0790406711371249E-2"/>
+                  <c:y val="-1.8650864831581012E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-547B-4278-BC18-552059D77641}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.2298028578812881E-3"/>
-                  <c:y val="-1.9452068702343527E-2"/>
+                  <c:x val="-3.912563649670147E-2"/>
+                  <c:y val="-3.2774122082393185E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1878,8 +2004,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.960862000516902E-2"/>
-                  <c:y val="-4.1683004362164752E-2"/>
+                  <c:x val="-8.6979050334242664E-2"/>
+                  <c:y val="-7.5208363548410883E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1902,6 +2028,48 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-2E8A-476E-9DD6-113B60E24F1B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5159263176677851E-2"/>
+                  <c:y val="-2.3979683354889873E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-547B-4278-BC18-552059D77641}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.4895794272887373E-2"/>
+                  <c:y val="-2.3979683354889897E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-547B-4278-BC18-552059D77641}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2535,6 +2703,90 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.6058186563306494E-2"/>
+                  <c:y val="-2.7044319192658348E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-D96D-4DEC-8BD0-1A8480D67B20}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.0735066629752394E-2"/>
+                  <c:y val="-2.4585744720598497E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-D96D-4DEC-8BD0-1A8480D67B20}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.0735066629752318E-2"/>
+                  <c:y val="-2.9502893664718199E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-D96D-4DEC-8BD0-1A8480D67B20}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.1960177679339524E-3"/>
+                  <c:y val="-2.4585744720598497E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-D96D-4DEC-8BD0-1A8480D67B20}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2618,16 +2870,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.67</c:v>
+                  <c:v>0.76160000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.66</c:v>
+                  <c:v>0.76319999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.68</c:v>
+                  <c:v>0.76859999999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.69140000000000001</c:v>
+                  <c:v>0.76180000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2679,11 +2931,32 @@
           </c:marker>
           <c:dLbls>
             <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.9911173237356053E-2"/>
+                  <c:y val="1.2292872360299203E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-D96D-4DEC-8BD0-1A8480D67B20}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.7127102165620299E-2"/>
-                  <c:y val="-2.9502893664718245E-2"/>
+                  <c:x val="-2.0490044419834878E-2"/>
+                  <c:y val="-1.7210021304418947E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -2842,6 +3115,27 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.8107191005290006E-2"/>
+                  <c:y val="-1.2292872360299294E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-D96D-4DEC-8BD0-1A8480D67B20}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2986,6 +3280,27 @@
           </c:marker>
           <c:dLbls>
             <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.6058186563306494E-2"/>
+                  <c:y val="-9.8342978882393992E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-D96D-4DEC-8BD0-1A8480D67B20}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
@@ -3024,6 +3339,27 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000006-9304-4464-8AB4-F0CEBDE6DDCB}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.2294026651900927E-2"/>
+                  <c:y val="2.212717024853865E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-D96D-4DEC-8BD0-1A8480D67B20}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -17156,9 +17492,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18591,8 +18927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57290BA2-B033-4EDB-8465-0445A2C8ADE5}">
   <dimension ref="B2:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="S62" sqref="S62"/>
+    <sheetView tabSelected="1" topLeftCell="J34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z60" sqref="Z60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -18800,7 +19136,7 @@
       <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>0.72470000000000001</v>
       </c>
       <c r="D11" s="7">
@@ -18817,17 +19153,17 @@
       <c r="B12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="7">
-        <v>0.67</v>
-      </c>
-      <c r="D12" s="7">
-        <v>0.66</v>
-      </c>
-      <c r="E12" s="7">
-        <v>0.68</v>
-      </c>
-      <c r="F12" s="7">
-        <v>0.69140000000000001</v>
+      <c r="C12" s="8">
+        <v>0.76160000000000005</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.76319999999999999</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.76859999999999995</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.76180000000000003</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.4">
@@ -18878,7 +19214,7 @@
       <c r="E15" s="7">
         <v>0.70199999999999996</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <v>0.75960000000000005</v>
       </c>
       <c r="G15" s="1"/>
@@ -19386,25 +19722,25 @@
       <c r="B62" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C62" s="7">
-        <v>0.70199999999999996</v>
-      </c>
-      <c r="D62" s="7">
-        <v>0.70199999999999996</v>
+      <c r="C62" s="8">
+        <v>0.76229999999999998</v>
+      </c>
+      <c r="D62" s="8">
+        <v>0.75819999999999999</v>
       </c>
       <c r="E62" s="7">
-        <v>0.67020000000000002</v>
-      </c>
-      <c r="F62" s="7">
+        <v>0.74919999999999998</v>
+      </c>
+      <c r="F62" s="8">
         <v>0.76</v>
       </c>
       <c r="G62" s="7">
-        <v>0.67020000000000002</v>
+        <v>0.75370000000000004</v>
       </c>
       <c r="H62" s="7">
-        <v>0.69148900000000002</v>
-      </c>
-      <c r="I62" s="7">
+        <v>0.75139999999999996</v>
+      </c>
+      <c r="I62" s="8">
         <v>0.76180000000000003</v>
       </c>
     </row>
@@ -19464,16 +19800,16 @@
       <c r="B65" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C65" s="8">
+      <c r="C65" s="7">
         <v>0.75319999999999998</v>
       </c>
-      <c r="D65" s="8">
+      <c r="D65" s="7">
         <v>0.74780000000000002</v>
       </c>
-      <c r="E65" s="8">
+      <c r="E65" s="7">
         <v>0.75139999999999996</v>
       </c>
-      <c r="F65" s="8">
+      <c r="F65" s="7">
         <v>0.74550000000000005</v>
       </c>
       <c r="G65" s="8">
@@ -19482,7 +19818,7 @@
       <c r="H65" s="8">
         <v>0.76590000000000003</v>
       </c>
-      <c r="I65" s="8">
+      <c r="I65" s="7">
         <v>0.75960000000000005</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mean shap value metrci update
</commit_message>
<xml_diff>
--- a/final_project/Metric.xlsx
+++ b/final_project/Metric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\22-1_multivariate\final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361FD40E-E11A-4FB6-BC28-B617C46B93B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D2B094-8C76-453F-B3AA-80E16FEC0421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{387F913E-4B8E-4F70-9082-430D9D091FEF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{387F913E-4B8E-4F70-9082-430D9D091FEF}"/>
   </bookViews>
   <sheets>
     <sheet name="specificity" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="acc" sheetId="3" r:id="rId3"/>
     <sheet name="AUC" sheetId="4" r:id="rId4"/>
     <sheet name="pvalue" sheetId="5" r:id="rId5"/>
+    <sheet name="hyperparams" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="57">
   <si>
     <t>logistic regression</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -199,6 +200,46 @@
   </si>
   <si>
     <t>PPIantacid</t>
+  </si>
+  <si>
+    <t>Classifier</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Random Forest</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gradient Boosting</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hyper parameters</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MLP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SVM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cost (c)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>learning rate, number of estimators</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of parameters, max depth</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of layers and hidden units</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3113,50 +3154,6 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-D96D-4DEC-8BD0-1A8480D67B20}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:numFmt formatCode="#,##0.000_);[Red]\(#,##0.000\)" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="0">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr algn="ctr">
-                    <a:defRPr lang="en-US" altLang="ko-KR" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="75000"/>
-                          <a:lumOff val="25000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="ko-KR"/>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000000-0F23-4DD1-9D81-FA543C566807}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -19497,13 +19494,13 @@
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>10</v>
       </c>
@@ -19520,7 +19517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -19540,7 +19537,7 @@
         <v>0.745</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -19560,7 +19557,7 @@
         <v>0.80799999999999905</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -19580,7 +19577,7 @@
         <v>0.80799999999999905</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>10</v>
       </c>
@@ -19594,7 +19591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -19611,7 +19608,7 @@
         <v>0.745</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -19628,7 +19625,7 @@
         <v>0.80799999999999905</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -19648,7 +19645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>10</v>
       </c>
@@ -19665,7 +19662,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -19686,7 +19683,7 @@
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -19707,7 +19704,7 @@
       </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -19728,7 +19725,7 @@
       </c>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -19749,7 +19746,7 @@
       </c>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -19770,7 +19767,7 @@
       </c>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -19807,13 +19804,13 @@
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.59765625" customWidth="1"/>
-    <col min="2" max="2" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.625" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>10</v>
       </c>
@@ -19827,7 +19824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -19845,7 +19842,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -19863,7 +19860,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -19881,7 +19878,7 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>10</v>
       </c>
@@ -19895,7 +19892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -19913,7 +19910,7 @@
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -19931,7 +19928,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -19949,7 +19946,7 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>10</v>
       </c>
@@ -19966,7 +19963,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -19986,7 +19983,7 @@
         <v>0.57399999999999995</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -20006,7 +20003,7 @@
         <v>0.57399999999999995</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -20026,7 +20023,7 @@
         <v>0.57399999999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -20046,7 +20043,7 @@
         <v>0.57399999999999995</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -20066,7 +20063,7 @@
         <v>0.57399999999999995</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -20101,14 +20098,14 @@
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="13.19921875" customWidth="1"/>
-    <col min="14" max="14" width="17.09765625" customWidth="1"/>
+    <col min="3" max="3" width="13.25" customWidth="1"/>
+    <col min="14" max="14" width="17.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>10</v>
       </c>
@@ -20122,7 +20119,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -20139,7 +20136,7 @@
         <v>0.65949999999999998</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -20156,7 +20153,7 @@
         <v>0.69099999999999995</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -20173,7 +20170,7 @@
         <v>0.69099999999999995</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>10</v>
       </c>
@@ -20187,7 +20184,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -20204,7 +20201,7 @@
         <v>0.65949999999999998</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -20221,7 +20218,7 @@
         <v>0.69099999999999995</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -20238,7 +20235,7 @@
         <v>0.69099999999999995</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>10</v>
       </c>
@@ -20255,7 +20252,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>0</v>
       </c>
@@ -20275,7 +20272,7 @@
         <v>0.65949999999999998</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>1</v>
       </c>
@@ -20295,7 +20292,7 @@
         <v>0.69099999999999995</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -20315,7 +20312,7 @@
         <v>0.69099999999999995</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>8</v>
       </c>
@@ -20335,7 +20332,7 @@
         <v>0.65949999999999998</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>6</v>
       </c>
@@ -20355,7 +20352,7 @@
         <v>0.69099999999999995</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>7</v>
       </c>
@@ -20375,7 +20372,7 @@
         <v>0.69099999999999995</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -20385,7 +20382,7 @@
       <c r="L26" s="4"/>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -20395,7 +20392,7 @@
       <c r="L27" s="4"/>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -20405,7 +20402,7 @@
       <c r="L28" s="4"/>
       <c r="N28" s="5"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -20415,7 +20412,7 @@
       <c r="L29" s="4"/>
       <c r="N29" s="5"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -20425,7 +20422,7 @@
       <c r="L30" s="4"/>
       <c r="N30" s="5"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -20435,7 +20432,7 @@
       <c r="L31" s="4"/>
       <c r="N31" s="5"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -20445,7 +20442,7 @@
       <c r="L32" s="4"/>
       <c r="N32" s="5"/>
     </row>
-    <row r="33" spans="4:14" x14ac:dyDescent="0.4">
+    <row r="33" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -20455,7 +20452,7 @@
       <c r="L33" s="4"/>
       <c r="N33" s="5"/>
     </row>
-    <row r="34" spans="4:14" x14ac:dyDescent="0.4">
+    <row r="34" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -20464,7 +20461,7 @@
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
     </row>
-    <row r="35" spans="4:14" x14ac:dyDescent="0.4">
+    <row r="35" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -20473,7 +20470,7 @@
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
     </row>
-    <row r="36" spans="4:14" x14ac:dyDescent="0.4">
+    <row r="36" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -20483,7 +20480,7 @@
       <c r="L36" s="4"/>
       <c r="N36" s="5"/>
     </row>
-    <row r="37" spans="4:14" x14ac:dyDescent="0.4">
+    <row r="37" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -20492,7 +20489,7 @@
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
     </row>
-    <row r="38" spans="4:14" x14ac:dyDescent="0.4">
+    <row r="38" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -20501,7 +20498,7 @@
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
     </row>
-    <row r="39" spans="4:14" x14ac:dyDescent="0.4">
+    <row r="39" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
@@ -20510,7 +20507,7 @@
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
     </row>
-    <row r="40" spans="4:14" x14ac:dyDescent="0.4">
+    <row r="40" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
@@ -20519,7 +20516,7 @@
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
     </row>
-    <row r="41" spans="4:14" x14ac:dyDescent="0.4">
+    <row r="41" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -20528,7 +20525,7 @@
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
     </row>
-    <row r="42" spans="4:14" x14ac:dyDescent="0.4">
+    <row r="42" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
@@ -20537,17 +20534,17 @@
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
     </row>
-    <row r="43" spans="4:14" x14ac:dyDescent="0.4">
+    <row r="43" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="4:14" x14ac:dyDescent="0.4">
+    <row r="44" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="4:14" x14ac:dyDescent="0.4">
+    <row r="45" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
@@ -20563,17 +20560,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57290BA2-B033-4EDB-8465-0445A2C8ADE5}">
   <dimension ref="B2:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH24" sqref="AH24"/>
+    <sheetView topLeftCell="A9" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Y63" sqref="Y63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.19921875" customWidth="1"/>
+    <col min="2" max="2" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:9" ht="33" x14ac:dyDescent="0.3">
       <c r="B2" s="6"/>
       <c r="C2" s="6">
         <v>10</v>
@@ -20597,7 +20594,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>12</v>
       </c>
@@ -20623,7 +20620,7 @@
         <v>0.66359999999999997</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>13</v>
       </c>
@@ -20649,7 +20646,7 @@
         <v>0.76180000000000003</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
@@ -20675,7 +20672,7 @@
         <v>0.70209999999999995</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
@@ -20701,7 +20698,7 @@
         <v>0.64639999999999997</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>16</v>
       </c>
@@ -20727,7 +20724,7 @@
         <v>0.75960000000000005</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
@@ -20753,7 +20750,7 @@
         <v>0.68620000000000003</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:9" ht="33" x14ac:dyDescent="0.3">
       <c r="B10" s="6"/>
       <c r="C10" s="6">
         <v>10</v>
@@ -20768,7 +20765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
@@ -20785,7 +20782,7 @@
         <v>0.66359999999999997</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
         <v>13</v>
       </c>
@@ -20802,7 +20799,7 @@
         <v>0.76180000000000003</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>14</v>
       </c>
@@ -20819,7 +20816,7 @@
         <v>0.72829999999999995</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
         <v>15</v>
       </c>
@@ -20837,7 +20834,7 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="s">
         <v>16</v>
       </c>
@@ -20855,7 +20852,7 @@
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>23</v>
       </c>
@@ -20873,7 +20870,7 @@
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>10</v>
       </c>
@@ -20890,7 +20887,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>0</v>
       </c>
@@ -20910,7 +20907,7 @@
         <v>0.66359999999999997</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>1</v>
       </c>
@@ -20930,7 +20927,7 @@
         <v>0.75960000000000005</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>2</v>
       </c>
@@ -20950,7 +20947,7 @@
         <v>0.76180000000000003</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>8</v>
       </c>
@@ -20970,7 +20967,7 @@
         <v>0.66359999999999997</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>6</v>
       </c>
@@ -20990,7 +20987,7 @@
         <v>0.75960000000000005</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>7</v>
       </c>
@@ -21010,7 +21007,7 @@
         <v>0.69140000000000001</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:9" ht="33" x14ac:dyDescent="0.3">
       <c r="B32" s="6"/>
       <c r="C32" s="6">
         <v>10</v>
@@ -21034,7 +21031,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="7" t="s">
         <v>12</v>
       </c>
@@ -21060,7 +21057,7 @@
         <v>0.66359999999999997</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="7" t="s">
         <v>13</v>
       </c>
@@ -21086,7 +21083,7 @@
         <v>0.76180000000000003</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="7" t="s">
         <v>14</v>
       </c>
@@ -21112,7 +21109,7 @@
         <v>0.70209999999999995</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" s="7" t="s">
         <v>15</v>
       </c>
@@ -21138,7 +21135,7 @@
         <v>0.64639999999999997</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37" s="7" t="s">
         <v>16</v>
       </c>
@@ -21164,7 +21161,7 @@
         <v>0.75960000000000005</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38" s="7" t="s">
         <v>18</v>
       </c>
@@ -21190,7 +21187,7 @@
         <v>0.66359999999999997</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39" s="7" t="s">
         <v>19</v>
       </c>
@@ -21216,7 +21213,7 @@
         <v>0.69140000000000001</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40" s="7" t="s">
         <v>20</v>
       </c>
@@ -21242,7 +21239,7 @@
         <v>0.70209999999999995</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B41" s="7" t="s">
         <v>21</v>
       </c>
@@ -21268,7 +21265,7 @@
         <v>0.64639999999999997</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42" s="7" t="s">
         <v>22</v>
       </c>
@@ -21294,7 +21291,7 @@
         <v>0.75960000000000005</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="8"/>
@@ -21304,7 +21301,7 @@
       <c r="H44" s="8"/>
       <c r="I44" s="7"/>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="60" spans="2:9" ht="33" x14ac:dyDescent="0.3">
       <c r="B60" s="6"/>
       <c r="C60" s="6">
         <v>10</v>
@@ -21328,7 +21325,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B61" s="7" t="s">
         <v>12</v>
       </c>
@@ -21354,7 +21351,7 @@
         <v>0.66359999999999997</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B62" s="7" t="s">
         <v>13</v>
       </c>
@@ -21380,7 +21377,7 @@
         <v>0.76180000000000003</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B63" s="7" t="s">
         <v>14</v>
       </c>
@@ -21406,7 +21403,7 @@
         <v>0.72829999999999995</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B64" s="7" t="s">
         <v>15</v>
       </c>
@@ -21432,7 +21429,7 @@
         <v>0.64639999999999997</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B65" s="7" t="s">
         <v>16</v>
       </c>
@@ -21458,7 +21455,7 @@
         <v>0.75960000000000005</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B66" s="7" t="s">
         <v>18</v>
       </c>
@@ -21484,7 +21481,7 @@
         <v>0.66359999999999997</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B67" s="7" t="s">
         <v>19</v>
       </c>
@@ -21510,7 +21507,7 @@
         <v>0.69140000000000001</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B68" s="7" t="s">
         <v>20</v>
       </c>
@@ -21536,7 +21533,7 @@
         <v>0.70209999999999995</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B69" s="7" t="s">
         <v>21</v>
       </c>
@@ -21562,7 +21559,7 @@
         <v>0.64639999999999997</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B70" s="7" t="s">
         <v>22</v>
       </c>
@@ -21588,7 +21585,7 @@
         <v>0.75960000000000005</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
       <c r="D72" s="8"/>
@@ -21609,13 +21606,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9686A57-AD2D-4E61-A677-8F29A20E8725}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>25</v>
       </c>
@@ -21626,7 +21623,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>28</v>
       </c>
@@ -21637,7 +21634,7 @@
         <v>7.6799999999999996E-11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>28</v>
       </c>
@@ -21648,7 +21645,7 @@
         <v>4.8999999999999996E-10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>28</v>
       </c>
@@ -21659,7 +21656,7 @@
         <v>1.0600000000000001E-9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>28</v>
       </c>
@@ -21670,7 +21667,7 @@
         <v>2.2600000000000001E-8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>28</v>
       </c>
@@ -21681,7 +21678,7 @@
         <v>9.879999999999999E-7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>34</v>
       </c>
@@ -21692,7 +21689,7 @@
         <v>1.01E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>28</v>
       </c>
@@ -21703,7 +21700,7 @@
         <v>8.9599999999999999E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>28</v>
       </c>
@@ -21714,7 +21711,7 @@
         <v>1.2819999999999999E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>34</v>
       </c>
@@ -21725,7 +21722,7 @@
         <v>8.7989999999999995E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>28</v>
       </c>
@@ -21736,7 +21733,7 @@
         <v>1.8303E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>34</v>
       </c>
@@ -21747,7 +21744,7 @@
         <v>1.8454000000000002E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>28</v>
       </c>
@@ -21758,7 +21755,7 @@
         <v>2.2189E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>34</v>
       </c>
@@ -21769,7 +21766,7 @@
         <v>2.3706000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>34</v>
       </c>
@@ -21780,7 +21777,7 @@
         <v>3.3569000000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>34</v>
       </c>
@@ -21791,7 +21788,7 @@
         <v>4.0586999999999998E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>28</v>
       </c>
@@ -21802,7 +21799,7 @@
         <v>4.2002999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>28</v>
       </c>
@@ -21818,4 +21815,64 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{109BB56C-276F-4861-8913-920E4A39C083}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="37.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>